<commit_message>
Filtro de separacion entre horas en un mismo día
</commit_message>
<xml_diff>
--- a/jesus/HorariosGII(24-25).xlsx
+++ b/jesus/HorariosGII(24-25).xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="1AGII" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,6 @@
     <sheet name="4GII(SI)" sheetId="23" state="visible" r:id="rId24"/>
     <sheet name="4GII(TI)" sheetId="24" state="visible" r:id="rId25"/>
     <sheet name="4GII(Com)" sheetId="25" state="visible" r:id="rId26"/>
-    <sheet name="Hoja26" sheetId="26" state="visible" r:id="rId27"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">1AGII!$A$1:$R$62</definedName>
@@ -57,7 +56,7 @@
     <definedName function="false" hidden="false" localSheetId="24" name="_xlnm.Print_Area" vbProcedure="false">'4GII(Com)'!$A$1:$M$30</definedName>
     <definedName function="false" hidden="false" localSheetId="21" name="_xlnm.Print_Area" vbProcedure="false">'4GII(CSI)'!$A$1:$O$61</definedName>
     <definedName function="false" hidden="false" localSheetId="19" name="_xlnm.Print_Area" vbProcedure="false">'4GII(IC)'!$A$1:$M$64</definedName>
-    <definedName function="false" hidden="false" localSheetId="20" name="_xlnm.Print_Area" vbProcedure="false">'4GII(IS)'!$A$1:$P$62</definedName>
+    <definedName function="false" hidden="false" localSheetId="20" name="_xlnm.Print_Area" vbProcedure="false">'4GII(IS)'!$A$2:$P$62</definedName>
     <definedName function="false" hidden="false" localSheetId="22" name="_xlnm.Print_Area" vbProcedure="false">'4GII(SI)'!$A$1:$M$61</definedName>
     <definedName function="false" hidden="false" localSheetId="23" name="_xlnm.Print_Area" vbProcedure="false">'4GII(TI)'!$A$1:$O$62</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">#REF!</definedName>
@@ -93,7 +92,7 @@
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm.Print_Area_0" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm.Print_Area_0" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="19" name="_xlnm.Print_Area_0" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="20" name="_xlnm.Print_Area" vbProcedure="false">'4GII(IS)'!$A$2:$P$62</definedName>
+    <definedName function="false" hidden="false" localSheetId="20" name="_xlnm.Print_Area" vbProcedure="false">'4GII(IS)'!$A$1:$P$62</definedName>
     <definedName function="false" hidden="false" localSheetId="20" name="_xlnm.Print_Area_0_0" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="21" name="_xlnm.Print_Area_0" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="21" name="_xlnm.Print_Area_0_0" vbProcedure="false">#REF!</definedName>
@@ -111,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3561" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3506" uniqueCount="695">
   <si>
     <t xml:space="preserve">1º A Grado en Ingeniería Informática</t>
   </si>
@@ -2061,25 +2060,25 @@
     <t xml:space="preserve">DGP. Dirección y Gestión de Proyectos.</t>
   </si>
   <si>
-    <t xml:space="preserve">MDA1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DBA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DGP3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DGP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MDA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DBA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DGP4</t>
+    <t xml:space="preserve">MDA (A1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DBA (A2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DGP (A3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DGP (A1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDA (A2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DBA (A3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DGP (A4)</t>
   </si>
   <si>
     <t xml:space="preserve">MDA. Metodologías de Desarrollo Ágil.</t>
@@ -2097,13 +2096,13 @@
     <t xml:space="preserve">DBA</t>
   </si>
   <si>
-    <t xml:space="preserve">DBA1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DGP2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MDA3</t>
+    <t xml:space="preserve">DBA (A1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DGP (A2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDA (A3)</t>
   </si>
   <si>
     <t xml:space="preserve">LP. Lógica y Programación.</t>
@@ -2362,102 +2361,6 @@
   </si>
   <si>
     <t xml:space="preserve">4º Grado en Ingeniería Informática (Formación Complementaria)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIMER SEMESTRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEGUNDO SEMESTRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAÑANA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TARDE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INFORMÁTICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1ABC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1DE(F)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2ABC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3ABCD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 (todas las menciones)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4(todas las menciones)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TELECOMUNICACIONES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 (todas las menciones)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOBLES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1ADE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1MAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2MAT 2ADE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3MAT 3ADE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MASTER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1INF 1TEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2TEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 grupos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 grupos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 grupos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 grupos</t>
   </si>
 </sst>
 </file>
@@ -2469,7 +2372,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00\ %"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2659,6 +2562,30 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -4686,7 +4613,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="687">
+  <cellXfs count="691">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7183,15 +7110,31 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="61" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="7" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="60" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="7" borderId="65" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7199,6 +7142,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7211,7 +7158,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7403,7 +7350,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="140" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="32" fillId="0" borderId="140" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7429,10 +7376,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="196" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -7515,8 +7458,8 @@
   </sheetPr>
   <dimension ref="A2:R61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="S:S B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9163,8 +9106,8 @@
   </sheetPr>
   <dimension ref="A2:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L45" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R57" activeCellId="1" sqref="S:S R57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10856,8 +10799,8 @@
   </sheetPr>
   <dimension ref="A2:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R18" activeCellId="1" sqref="S:S R18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R18" activeCellId="0" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11757,8 +11700,8 @@
   </sheetPr>
   <dimension ref="A2:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R22" activeCellId="1" sqref="S:S R22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R22" activeCellId="0" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12655,8 +12598,8 @@
   </sheetPr>
   <dimension ref="A2:M29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M22" activeCellId="1" sqref="S:S M22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M22" activeCellId="0" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13311,8 +13254,8 @@
   </sheetPr>
   <dimension ref="A2:O29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O18" activeCellId="1" sqref="S:S O18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O18" activeCellId="0" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13964,8 +13907,8 @@
   </sheetPr>
   <dimension ref="A2:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H12" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M20" activeCellId="1" sqref="S:S M20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H12" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14638,8 +14581,8 @@
   </sheetPr>
   <dimension ref="A2:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K17" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R38" activeCellId="1" sqref="S:S R38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K17" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R38" activeCellId="0" sqref="R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15534,8 +15477,8 @@
   </sheetPr>
   <dimension ref="A2:S29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S21" activeCellId="0" sqref="S:S"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S21" activeCellId="0" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16390,8 +16333,8 @@
   </sheetPr>
   <dimension ref="A2:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R25" activeCellId="1" sqref="S:S R25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J7" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R25" activeCellId="0" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17277,8 +17220,8 @@
   </sheetPr>
   <dimension ref="A2:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R21" activeCellId="1" sqref="S:S R21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R21" activeCellId="0" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18256,8 +18199,8 @@
   </sheetPr>
   <dimension ref="A2:R61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S:S"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19858,8 +19801,8 @@
   </sheetPr>
   <dimension ref="A2:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M4" activeCellId="1" sqref="S:S M4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20468,7 +20411,7 @@
       <c r="K33" s="71"/>
       <c r="M33" s="315"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>562</v>
       </c>
@@ -20483,7 +20426,7 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="22.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>53</v>
       </c>
@@ -21278,8 +21221,8 @@
   </sheetPr>
   <dimension ref="A2:P62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P42" activeCellId="1" sqref="S:S P42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21478,13 +21421,13 @@
         <v>592</v>
       </c>
       <c r="G9" s="529"/>
-      <c r="H9" s="47" t="s">
+      <c r="H9" s="624" t="s">
         <v>594</v>
       </c>
       <c r="I9" s="89" t="s">
         <v>595</v>
       </c>
-      <c r="J9" s="90" t="s">
+      <c r="J9" s="625" t="s">
         <v>596</v>
       </c>
       <c r="K9" s="47" t="s">
@@ -21546,10 +21489,10 @@
       <c r="A11" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="624" t="s">
+      <c r="B11" s="626" t="s">
         <v>590</v>
       </c>
-      <c r="C11" s="624"/>
+      <c r="C11" s="626"/>
       <c r="D11" s="27" t="s">
         <v>591</v>
       </c>
@@ -21558,22 +21501,22 @@
         <v>592</v>
       </c>
       <c r="G11" s="27"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="624" t="s">
         <v>594</v>
       </c>
       <c r="I11" s="89" t="s">
         <v>595</v>
       </c>
-      <c r="J11" s="90" t="s">
+      <c r="J11" s="625" t="s">
         <v>596</v>
       </c>
-      <c r="K11" s="47" t="s">
+      <c r="K11" s="624" t="s">
         <v>597</v>
       </c>
-      <c r="L11" s="89" t="s">
+      <c r="L11" s="627" t="s">
         <v>598</v>
       </c>
-      <c r="M11" s="89" t="s">
+      <c r="M11" s="627" t="s">
         <v>599</v>
       </c>
       <c r="N11" s="283" t="s">
@@ -21584,10 +21527,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="25"/>
-      <c r="B12" s="625" t="s">
+      <c r="B12" s="628" t="s">
         <v>167</v>
       </c>
-      <c r="C12" s="625"/>
+      <c r="C12" s="628"/>
       <c r="D12" s="153" t="s">
         <v>500</v>
       </c>
@@ -21624,10 +21567,10 @@
       <c r="A13" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="626" t="s">
+      <c r="B13" s="629" t="s">
         <v>590</v>
       </c>
-      <c r="C13" s="626"/>
+      <c r="C13" s="629"/>
       <c r="D13" s="157" t="s">
         <v>591</v>
       </c>
@@ -21644,10 +21587,10 @@
       <c r="K13" s="47" t="s">
         <v>606</v>
       </c>
-      <c r="L13" s="89" t="s">
+      <c r="L13" s="627" t="s">
         <v>607</v>
       </c>
-      <c r="M13" s="89" t="s">
+      <c r="M13" s="627" t="s">
         <v>608</v>
       </c>
       <c r="N13" s="283"/>
@@ -21658,10 +21601,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="46"/>
-      <c r="B14" s="625" t="s">
+      <c r="B14" s="628" t="s">
         <v>167</v>
       </c>
-      <c r="C14" s="625"/>
+      <c r="C14" s="628"/>
       <c r="D14" s="153" t="s">
         <v>500</v>
       </c>
@@ -21670,11 +21613,11 @@
         <v>218</v>
       </c>
       <c r="G14" s="153"/>
-      <c r="H14" s="153" t="s">
+      <c r="H14" s="630" t="s">
         <v>589</v>
       </c>
-      <c r="I14" s="153"/>
-      <c r="J14" s="153"/>
+      <c r="I14" s="630"/>
+      <c r="J14" s="630"/>
       <c r="K14" s="17" t="s">
         <v>603</v>
       </c>
@@ -21694,8 +21637,8 @@
       </c>
       <c r="B15" s="620"/>
       <c r="C15" s="620"/>
-      <c r="D15" s="627"/>
-      <c r="E15" s="627"/>
+      <c r="D15" s="631"/>
+      <c r="E15" s="631"/>
       <c r="F15" s="620"/>
       <c r="G15" s="620"/>
       <c r="H15" s="27" t="s">
@@ -21703,13 +21646,13 @@
       </c>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
-      <c r="K15" s="47" t="s">
+      <c r="K15" s="632" t="s">
         <v>606</v>
       </c>
       <c r="L15" s="89" t="s">
         <v>607</v>
       </c>
-      <c r="M15" s="89" t="s">
+      <c r="M15" s="627" t="s">
         <v>608</v>
       </c>
       <c r="N15" s="283"/>
@@ -21768,7 +21711,7 @@
       <c r="A18" s="477" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="628"/>
+      <c r="B18" s="633"/>
       <c r="C18" s="55"/>
       <c r="D18" s="111"/>
       <c r="E18" s="55"/>
@@ -21824,7 +21767,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="478"/>
-      <c r="B21" s="629"/>
+      <c r="B21" s="634"/>
       <c r="C21" s="598"/>
       <c r="D21" s="597"/>
       <c r="E21" s="598"/>
@@ -21862,7 +21805,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="478"/>
-      <c r="B23" s="629"/>
+      <c r="B23" s="634"/>
       <c r="C23" s="598"/>
       <c r="D23" s="597"/>
       <c r="E23" s="598"/>
@@ -21898,7 +21841,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="478"/>
-      <c r="B25" s="629"/>
+      <c r="B25" s="634"/>
       <c r="C25" s="598"/>
       <c r="D25" s="597"/>
       <c r="E25" s="598"/>
@@ -21934,7 +21877,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="478"/>
-      <c r="B27" s="629"/>
+      <c r="B27" s="634"/>
       <c r="C27" s="598"/>
       <c r="D27" s="597"/>
       <c r="E27" s="598"/>
@@ -21972,9 +21915,9 @@
       <c r="A29" s="64"/>
       <c r="B29" s="162"/>
       <c r="C29" s="163"/>
-      <c r="D29" s="630"/>
+      <c r="D29" s="635"/>
       <c r="E29" s="163"/>
-      <c r="F29" s="630"/>
+      <c r="F29" s="635"/>
       <c r="G29" s="163"/>
       <c r="H29" s="65"/>
       <c r="I29" s="299"/>
@@ -22085,7 +22028,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
-      <c r="P35" s="631"/>
+      <c r="P35" s="636"/>
     </row>
     <row r="36" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="126"/>
@@ -22101,11 +22044,11 @@
         <v>4</v>
       </c>
       <c r="G36" s="109"/>
-      <c r="H36" s="632" t="s">
+      <c r="H36" s="637" t="s">
         <v>5</v>
       </c>
-      <c r="I36" s="632"/>
-      <c r="J36" s="632"/>
+      <c r="I36" s="637"/>
+      <c r="J36" s="637"/>
       <c r="K36" s="246" t="s">
         <v>6</v>
       </c>
@@ -22119,12 +22062,12 @@
       </c>
       <c r="B37" s="112"/>
       <c r="C37" s="55"/>
-      <c r="D37" s="633"/>
-      <c r="E37" s="633"/>
-      <c r="F37" s="634" t="s">
+      <c r="D37" s="638"/>
+      <c r="E37" s="638"/>
+      <c r="F37" s="639" t="s">
         <v>574</v>
       </c>
-      <c r="G37" s="634"/>
+      <c r="G37" s="639"/>
       <c r="H37" s="111"/>
       <c r="I37" s="431"/>
       <c r="J37" s="432"/>
@@ -22145,19 +22088,19 @@
       <c r="C38" s="88"/>
       <c r="D38" s="560"/>
       <c r="E38" s="560"/>
-      <c r="F38" s="635" t="s">
+      <c r="F38" s="640" t="s">
         <v>500</v>
       </c>
-      <c r="G38" s="635"/>
+      <c r="G38" s="640"/>
       <c r="H38" s="61"/>
       <c r="I38" s="434"/>
       <c r="J38" s="435"/>
-      <c r="K38" s="636" t="s">
+      <c r="K38" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L38" s="636"/>
-      <c r="M38" s="636"/>
-      <c r="N38" s="636"/>
+      <c r="L38" s="641"/>
+      <c r="M38" s="641"/>
+      <c r="N38" s="641"/>
       <c r="O38" s="81"/>
     </row>
     <row r="39" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22172,10 +22115,10 @@
         <v>613</v>
       </c>
       <c r="E39" s="39"/>
-      <c r="F39" s="634" t="s">
+      <c r="F39" s="639" t="s">
         <v>574</v>
       </c>
-      <c r="G39" s="634"/>
+      <c r="G39" s="639"/>
       <c r="H39" s="27" t="s">
         <v>614</v>
       </c>
@@ -22202,21 +22145,21 @@
         <v>167</v>
       </c>
       <c r="E40" s="155"/>
-      <c r="F40" s="635" t="s">
+      <c r="F40" s="640" t="s">
         <v>500</v>
       </c>
-      <c r="G40" s="635"/>
+      <c r="G40" s="640"/>
       <c r="H40" s="30" t="s">
         <v>36</v>
       </c>
       <c r="I40" s="30"/>
       <c r="J40" s="30"/>
-      <c r="K40" s="636" t="s">
+      <c r="K40" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L40" s="636"/>
-      <c r="M40" s="636"/>
-      <c r="N40" s="636"/>
+      <c r="L40" s="641"/>
+      <c r="M40" s="641"/>
+      <c r="N40" s="641"/>
       <c r="O40" s="33"/>
       <c r="P40" s="323"/>
     </row>
@@ -22271,12 +22214,12 @@
       </c>
       <c r="I42" s="30"/>
       <c r="J42" s="30"/>
-      <c r="K42" s="636" t="s">
+      <c r="K42" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L42" s="636"/>
-      <c r="M42" s="636"/>
-      <c r="N42" s="636"/>
+      <c r="L42" s="641"/>
+      <c r="M42" s="641"/>
+      <c r="N42" s="641"/>
       <c r="O42" s="33"/>
       <c r="P42" s="33"/>
     </row>
@@ -22329,12 +22272,12 @@
       </c>
       <c r="I44" s="621"/>
       <c r="J44" s="621"/>
-      <c r="K44" s="636" t="s">
+      <c r="K44" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L44" s="636"/>
-      <c r="M44" s="636"/>
-      <c r="N44" s="636"/>
+      <c r="L44" s="641"/>
+      <c r="M44" s="641"/>
+      <c r="N44" s="641"/>
       <c r="O44" s="33"/>
       <c r="P44" s="0"/>
     </row>
@@ -22389,12 +22332,12 @@
       </c>
       <c r="I46" s="621"/>
       <c r="J46" s="621"/>
-      <c r="K46" s="636" t="s">
+      <c r="K46" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L46" s="636"/>
-      <c r="M46" s="636"/>
-      <c r="N46" s="636"/>
+      <c r="L46" s="641"/>
+      <c r="M46" s="641"/>
+      <c r="N46" s="641"/>
       <c r="O46" s="81"/>
       <c r="P46" s="0"/>
     </row>
@@ -22437,12 +22380,12 @@
       <c r="H48" s="602"/>
       <c r="I48" s="106"/>
       <c r="J48" s="107"/>
-      <c r="K48" s="636" t="s">
+      <c r="K48" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L48" s="636"/>
-      <c r="M48" s="636"/>
-      <c r="N48" s="636"/>
+      <c r="L48" s="641"/>
+      <c r="M48" s="641"/>
+      <c r="N48" s="641"/>
       <c r="O48" s="81"/>
       <c r="P48" s="0"/>
     </row>
@@ -22857,8 +22800,8 @@
   </sheetPr>
   <dimension ref="A2:O62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J26" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O43" activeCellId="1" sqref="S:S O43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O43" activeCellId="0" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22872,21 +22815,21 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="637" t="s">
+      <c r="A2" s="642" t="s">
         <v>618</v>
       </c>
-      <c r="B2" s="637"/>
-      <c r="C2" s="637"/>
-      <c r="D2" s="637"/>
-      <c r="E2" s="637"/>
-      <c r="F2" s="637"/>
-      <c r="G2" s="637"/>
-      <c r="H2" s="637"/>
-      <c r="I2" s="637"/>
-      <c r="J2" s="637"/>
-      <c r="K2" s="637"/>
-      <c r="L2" s="637"/>
-      <c r="M2" s="637"/>
+      <c r="B2" s="642"/>
+      <c r="C2" s="642"/>
+      <c r="D2" s="642"/>
+      <c r="E2" s="642"/>
+      <c r="F2" s="642"/>
+      <c r="G2" s="642"/>
+      <c r="H2" s="642"/>
+      <c r="I2" s="642"/>
+      <c r="J2" s="642"/>
+      <c r="K2" s="642"/>
+      <c r="L2" s="642"/>
+      <c r="M2" s="642"/>
     </row>
     <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="583" t="s">
@@ -22906,11 +22849,11 @@
       <c r="M3" s="583"/>
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="638"/>
-      <c r="B4" s="639" t="s">
+      <c r="A4" s="643"/>
+      <c r="B4" s="644" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="639"/>
+      <c r="C4" s="644"/>
       <c r="D4" s="585" t="s">
         <v>3</v>
       </c>
@@ -22919,11 +22862,11 @@
         <v>4</v>
       </c>
       <c r="G4" s="586"/>
-      <c r="H4" s="639" t="s">
+      <c r="H4" s="644" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="639"/>
-      <c r="J4" s="639"/>
+      <c r="I4" s="644"/>
+      <c r="J4" s="644"/>
       <c r="K4" s="587" t="s">
         <v>6</v>
       </c>
@@ -22938,13 +22881,13 @@
       <c r="C5" s="10"/>
       <c r="D5" s="14"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="640"/>
-      <c r="G5" s="641"/>
-      <c r="H5" s="642" t="s">
+      <c r="F5" s="645"/>
+      <c r="G5" s="646"/>
+      <c r="H5" s="647" t="s">
         <v>619</v>
       </c>
-      <c r="I5" s="642"/>
-      <c r="J5" s="642"/>
+      <c r="I5" s="647"/>
+      <c r="J5" s="647"/>
       <c r="K5" s="47" t="s">
         <v>620</v>
       </c>
@@ -22960,7 +22903,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
-      <c r="B6" s="643"/>
+      <c r="B6" s="648"/>
       <c r="C6" s="421"/>
       <c r="D6" s="621"/>
       <c r="E6" s="621"/>
@@ -22990,10 +22933,10 @@
         <v>624</v>
       </c>
       <c r="C7" s="27"/>
-      <c r="D7" s="624" t="s">
+      <c r="D7" s="626" t="s">
         <v>625</v>
       </c>
-      <c r="E7" s="624"/>
+      <c r="E7" s="626"/>
       <c r="F7" s="529" t="s">
         <v>624</v>
       </c>
@@ -23023,19 +22966,19 @@
         <v>500</v>
       </c>
       <c r="C8" s="153"/>
-      <c r="D8" s="625" t="s">
+      <c r="D8" s="628" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="625"/>
+      <c r="E8" s="628"/>
       <c r="F8" s="621" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="621"/>
-      <c r="H8" s="644" t="s">
+      <c r="H8" s="649" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="644"/>
-      <c r="J8" s="644"/>
+      <c r="I8" s="649"/>
+      <c r="J8" s="649"/>
       <c r="K8" s="17" t="s">
         <v>35</v>
       </c>
@@ -23126,10 +23069,10 @@
         <v>632</v>
       </c>
       <c r="E11" s="529"/>
-      <c r="F11" s="624" t="s">
+      <c r="F11" s="626" t="s">
         <v>632</v>
       </c>
-      <c r="G11" s="624"/>
+      <c r="G11" s="626"/>
       <c r="H11" s="47" t="s">
         <v>627</v>
       </c>
@@ -23157,10 +23100,10 @@
         <v>64</v>
       </c>
       <c r="E12" s="621"/>
-      <c r="F12" s="625" t="s">
+      <c r="F12" s="628" t="s">
         <v>500</v>
       </c>
-      <c r="G12" s="625"/>
+      <c r="G12" s="628"/>
       <c r="H12" s="17" t="s">
         <v>45</v>
       </c>
@@ -23190,10 +23133,10 @@
         <v>632</v>
       </c>
       <c r="E13" s="529"/>
-      <c r="F13" s="624" t="s">
+      <c r="F13" s="626" t="s">
         <v>632</v>
       </c>
-      <c r="G13" s="624"/>
+      <c r="G13" s="626"/>
       <c r="H13" s="28" t="s">
         <v>633</v>
       </c>
@@ -23223,10 +23166,10 @@
         <v>64</v>
       </c>
       <c r="E14" s="621"/>
-      <c r="F14" s="625" t="s">
+      <c r="F14" s="628" t="s">
         <v>500</v>
       </c>
-      <c r="G14" s="625"/>
+      <c r="G14" s="628"/>
       <c r="H14" s="153" t="s">
         <v>68</v>
       </c>
@@ -23275,17 +23218,17 @@
     </row>
     <row r="16" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="49"/>
-      <c r="B16" s="645"/>
-      <c r="C16" s="645"/>
+      <c r="B16" s="650"/>
+      <c r="C16" s="650"/>
       <c r="D16" s="621"/>
       <c r="E16" s="621"/>
-      <c r="F16" s="645"/>
-      <c r="G16" s="645"/>
-      <c r="H16" s="644" t="s">
+      <c r="F16" s="650"/>
+      <c r="G16" s="650"/>
+      <c r="H16" s="649" t="s">
         <v>68</v>
       </c>
-      <c r="I16" s="644"/>
-      <c r="J16" s="644"/>
+      <c r="I16" s="649"/>
+      <c r="J16" s="649"/>
       <c r="K16" s="17" t="s">
         <v>65</v>
       </c>
@@ -23321,7 +23264,7 @@
       <c r="A18" s="477" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="628"/>
+      <c r="B18" s="633"/>
       <c r="C18" s="55"/>
       <c r="D18" s="111"/>
       <c r="E18" s="55"/>
@@ -23374,7 +23317,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="478"/>
-      <c r="B21" s="629"/>
+      <c r="B21" s="634"/>
       <c r="C21" s="598"/>
       <c r="D21" s="597"/>
       <c r="E21" s="598"/>
@@ -23410,7 +23353,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="478"/>
-      <c r="B23" s="629"/>
+      <c r="B23" s="634"/>
       <c r="C23" s="598"/>
       <c r="D23" s="597"/>
       <c r="E23" s="598"/>
@@ -23446,7 +23389,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="478"/>
-      <c r="B25" s="629"/>
+      <c r="B25" s="634"/>
       <c r="C25" s="598"/>
       <c r="D25" s="597"/>
       <c r="E25" s="598"/>
@@ -23482,7 +23425,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="478"/>
-      <c r="B27" s="629"/>
+      <c r="B27" s="634"/>
       <c r="C27" s="598"/>
       <c r="D27" s="597"/>
       <c r="E27" s="598"/>
@@ -23520,9 +23463,9 @@
       <c r="A29" s="64"/>
       <c r="B29" s="162"/>
       <c r="C29" s="163"/>
-      <c r="D29" s="630"/>
+      <c r="D29" s="635"/>
       <c r="E29" s="163"/>
-      <c r="F29" s="630"/>
+      <c r="F29" s="635"/>
       <c r="G29" s="163"/>
       <c r="H29" s="65"/>
       <c r="I29" s="299"/>
@@ -23556,7 +23499,7 @@
       <c r="L31" s="603"/>
       <c r="M31" s="603"/>
       <c r="N31" s="603"/>
-      <c r="O31" s="631"/>
+      <c r="O31" s="636"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="70"/>
@@ -23617,24 +23560,24 @@
       <c r="M35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="646"/>
+      <c r="A36" s="651"/>
       <c r="B36" s="75" t="s">
         <v>2</v>
       </c>
       <c r="C36" s="75"/>
-      <c r="D36" s="647" t="s">
+      <c r="D36" s="652" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="647"/>
+      <c r="E36" s="652"/>
       <c r="F36" s="75" t="s">
         <v>4</v>
       </c>
       <c r="G36" s="75"/>
-      <c r="H36" s="647" t="s">
+      <c r="H36" s="652" t="s">
         <v>5</v>
       </c>
-      <c r="I36" s="647"/>
-      <c r="J36" s="647"/>
+      <c r="I36" s="652"/>
+      <c r="J36" s="652"/>
       <c r="K36" s="75" t="s">
         <v>6</v>
       </c>
@@ -23672,18 +23615,18 @@
       <c r="C38" s="124"/>
       <c r="D38" s="61"/>
       <c r="E38" s="88"/>
-      <c r="F38" s="648" t="s">
+      <c r="F38" s="653" t="s">
         <v>500</v>
       </c>
-      <c r="G38" s="648"/>
+      <c r="G38" s="653"/>
       <c r="H38" s="621"/>
       <c r="I38" s="621"/>
       <c r="J38" s="621"/>
-      <c r="K38" s="636" t="s">
+      <c r="K38" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L38" s="636"/>
-      <c r="M38" s="636"/>
+      <c r="L38" s="641"/>
+      <c r="M38" s="641"/>
       <c r="N38" s="81"/>
       <c r="O38" s="323"/>
     </row>
@@ -23728,20 +23671,20 @@
         <v>500</v>
       </c>
       <c r="E40" s="153"/>
-      <c r="F40" s="648" t="s">
+      <c r="F40" s="653" t="s">
         <v>500</v>
       </c>
-      <c r="G40" s="648"/>
+      <c r="G40" s="653"/>
       <c r="H40" s="153" t="s">
         <v>77</v>
       </c>
       <c r="I40" s="153"/>
       <c r="J40" s="153"/>
-      <c r="K40" s="636" t="s">
+      <c r="K40" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L40" s="636"/>
-      <c r="M40" s="636"/>
+      <c r="L40" s="641"/>
+      <c r="M40" s="641"/>
       <c r="N40" s="33"/>
       <c r="O40" s="33"/>
     </row>
@@ -23795,11 +23738,11 @@
       </c>
       <c r="I42" s="153"/>
       <c r="J42" s="153"/>
-      <c r="K42" s="636" t="s">
+      <c r="K42" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L42" s="636"/>
-      <c r="M42" s="636"/>
+      <c r="L42" s="641"/>
+      <c r="M42" s="641"/>
       <c r="N42" s="33"/>
       <c r="O42" s="33"/>
     </row>
@@ -23851,11 +23794,11 @@
       </c>
       <c r="I44" s="621"/>
       <c r="J44" s="621"/>
-      <c r="K44" s="636" t="s">
+      <c r="K44" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L44" s="636"/>
-      <c r="M44" s="636"/>
+      <c r="L44" s="641"/>
+      <c r="M44" s="641"/>
       <c r="N44" s="33"/>
       <c r="O44" s="0"/>
     </row>
@@ -23909,11 +23852,11 @@
       </c>
       <c r="I46" s="621"/>
       <c r="J46" s="621"/>
-      <c r="K46" s="636" t="s">
+      <c r="K46" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L46" s="636"/>
-      <c r="M46" s="636"/>
+      <c r="L46" s="641"/>
+      <c r="M46" s="641"/>
       <c r="N46" s="81"/>
       <c r="O46" s="0"/>
     </row>
@@ -23955,11 +23898,11 @@
       <c r="H48" s="621"/>
       <c r="I48" s="621"/>
       <c r="J48" s="621"/>
-      <c r="K48" s="636" t="s">
+      <c r="K48" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L48" s="636"/>
-      <c r="M48" s="636"/>
+      <c r="L48" s="641"/>
+      <c r="M48" s="641"/>
       <c r="N48" s="81"/>
       <c r="O48" s="0"/>
     </row>
@@ -24356,8 +24299,8 @@
   </sheetPr>
   <dimension ref="A2:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M20" activeCellId="1" sqref="S:S M20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H42" activeCellId="0" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24402,48 +24345,48 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="584"/>
-      <c r="B4" s="649" t="s">
+      <c r="B4" s="654" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="649"/>
-      <c r="D4" s="650" t="s">
+      <c r="C4" s="654"/>
+      <c r="D4" s="655" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="650"/>
-      <c r="F4" s="649" t="s">
+      <c r="E4" s="655"/>
+      <c r="F4" s="654" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="649"/>
-      <c r="H4" s="650" t="s">
+      <c r="G4" s="654"/>
+      <c r="H4" s="655" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="650"/>
-      <c r="J4" s="649" t="s">
+      <c r="I4" s="655"/>
+      <c r="J4" s="654" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="649"/>
+      <c r="K4" s="654"/>
       <c r="M4" s="101"/>
     </row>
     <row r="5" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="651"/>
-      <c r="C5" s="651"/>
-      <c r="D5" s="633"/>
-      <c r="E5" s="633"/>
-      <c r="F5" s="652"/>
-      <c r="G5" s="653"/>
-      <c r="H5" s="654" t="s">
+      <c r="B5" s="656"/>
+      <c r="C5" s="656"/>
+      <c r="D5" s="638"/>
+      <c r="E5" s="638"/>
+      <c r="F5" s="657"/>
+      <c r="G5" s="658"/>
+      <c r="H5" s="659" t="s">
         <v>649</v>
       </c>
-      <c r="I5" s="655" t="s">
+      <c r="I5" s="660" t="s">
         <v>650</v>
       </c>
-      <c r="J5" s="654" t="s">
+      <c r="J5" s="659" t="s">
         <v>651</v>
       </c>
-      <c r="K5" s="656" t="s">
+      <c r="K5" s="661" t="s">
         <v>652</v>
       </c>
       <c r="M5" s="599" t="s">
@@ -24476,14 +24419,14 @@
       <c r="A7" s="208" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="657" t="s">
+      <c r="B7" s="662" t="s">
         <v>654</v>
       </c>
-      <c r="C7" s="657"/>
-      <c r="D7" s="658" t="s">
+      <c r="C7" s="662"/>
+      <c r="D7" s="663" t="s">
         <v>655</v>
       </c>
-      <c r="E7" s="658"/>
+      <c r="E7" s="663"/>
       <c r="F7" s="529" t="s">
         <v>656</v>
       </c>
@@ -24500,7 +24443,7 @@
       <c r="K7" s="454" t="s">
         <v>652</v>
       </c>
-      <c r="L7" s="659"/>
+      <c r="L7" s="664"/>
       <c r="M7" s="101" t="s">
         <v>657</v>
       </c>
@@ -24531,21 +24474,21 @@
       <c r="K8" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="L8" s="660"/>
+      <c r="L8" s="665"/>
       <c r="M8" s="33"/>
     </row>
     <row r="9" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="657" t="s">
+      <c r="B9" s="662" t="s">
         <v>654</v>
       </c>
-      <c r="C9" s="657"/>
-      <c r="D9" s="658" t="s">
+      <c r="C9" s="662"/>
+      <c r="D9" s="663" t="s">
         <v>655</v>
       </c>
-      <c r="E9" s="658"/>
+      <c r="E9" s="663"/>
       <c r="F9" s="529" t="s">
         <v>656</v>
       </c>
@@ -24558,7 +24501,7 @@
         <v>658</v>
       </c>
       <c r="K9" s="182"/>
-      <c r="L9" s="660"/>
+      <c r="L9" s="665"/>
       <c r="M9" s="595" t="s">
         <v>659</v>
       </c>
@@ -24596,10 +24539,10 @@
         <v>654</v>
       </c>
       <c r="C11" s="95"/>
-      <c r="D11" s="661" t="s">
+      <c r="D11" s="666" t="s">
         <v>655</v>
       </c>
-      <c r="E11" s="661"/>
+      <c r="E11" s="666"/>
       <c r="F11" s="27" t="s">
         <v>656</v>
       </c>
@@ -24648,10 +24591,10 @@
         <v>654</v>
       </c>
       <c r="C13" s="95"/>
-      <c r="D13" s="661" t="s">
+      <c r="D13" s="666" t="s">
         <v>655</v>
       </c>
-      <c r="E13" s="661"/>
+      <c r="E13" s="666"/>
       <c r="F13" s="27" t="s">
         <v>656</v>
       </c>
@@ -24702,12 +24645,12 @@
       <c r="A15" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="651"/>
-      <c r="C15" s="651"/>
-      <c r="D15" s="633"/>
-      <c r="E15" s="633"/>
-      <c r="F15" s="633"/>
-      <c r="G15" s="633"/>
+      <c r="B15" s="656"/>
+      <c r="C15" s="656"/>
+      <c r="D15" s="638"/>
+      <c r="E15" s="638"/>
+      <c r="F15" s="638"/>
+      <c r="G15" s="638"/>
       <c r="H15" s="26" t="s">
         <v>660</v>
       </c>
@@ -24725,8 +24668,8 @@
     </row>
     <row r="16" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="49"/>
-      <c r="B16" s="662"/>
-      <c r="C16" s="662"/>
+      <c r="B16" s="667"/>
+      <c r="C16" s="667"/>
       <c r="D16" s="560"/>
       <c r="E16" s="560"/>
       <c r="F16" s="530"/>
@@ -24735,7 +24678,7 @@
         <v>218</v>
       </c>
       <c r="I16" s="158"/>
-      <c r="J16" s="663" t="s">
+      <c r="J16" s="668" t="s">
         <v>167</v>
       </c>
       <c r="K16" s="328" t="s">
@@ -25008,7 +24951,7 @@
       <c r="K34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="664"/>
+      <c r="A35" s="669"/>
       <c r="B35" s="246" t="s">
         <v>2</v>
       </c>
@@ -25034,14 +24977,14 @@
       <c r="A36" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="665"/>
-      <c r="C36" s="666"/>
-      <c r="D36" s="667"/>
-      <c r="E36" s="668"/>
-      <c r="F36" s="634" t="s">
+      <c r="B36" s="670"/>
+      <c r="C36" s="671"/>
+      <c r="D36" s="672"/>
+      <c r="E36" s="673"/>
+      <c r="F36" s="639" t="s">
         <v>574</v>
       </c>
-      <c r="G36" s="634"/>
+      <c r="G36" s="639"/>
       <c r="H36" s="8"/>
       <c r="I36" s="144"/>
       <c r="J36" s="606" t="s">
@@ -25056,13 +24999,13 @@
     <row r="37" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="7"/>
       <c r="B37" s="171"/>
-      <c r="C37" s="669"/>
-      <c r="D37" s="670"/>
-      <c r="E37" s="671"/>
-      <c r="F37" s="635" t="s">
+      <c r="C37" s="674"/>
+      <c r="D37" s="675"/>
+      <c r="E37" s="676"/>
+      <c r="F37" s="640" t="s">
         <v>500</v>
       </c>
-      <c r="G37" s="635"/>
+      <c r="G37" s="640"/>
       <c r="H37" s="58"/>
       <c r="I37" s="124"/>
       <c r="J37" s="607" t="s">
@@ -25084,10 +25027,10 @@
         <v>667</v>
       </c>
       <c r="E38" s="27"/>
-      <c r="F38" s="634" t="s">
+      <c r="F38" s="639" t="s">
         <v>574</v>
       </c>
-      <c r="G38" s="634"/>
+      <c r="G38" s="639"/>
       <c r="H38" s="327" t="s">
         <v>667</v>
       </c>
@@ -25138,10 +25081,10 @@
         <v>667</v>
       </c>
       <c r="E40" s="27"/>
-      <c r="F40" s="657" t="s">
+      <c r="F40" s="662" t="s">
         <v>669</v>
       </c>
-      <c r="G40" s="657"/>
+      <c r="G40" s="662"/>
       <c r="H40" s="327" t="s">
         <v>667</v>
       </c>
@@ -25282,7 +25225,7 @@
         <v>669</v>
       </c>
       <c r="G46" s="27"/>
-      <c r="H46" s="672"/>
+      <c r="H46" s="677"/>
       <c r="I46" s="613"/>
       <c r="J46" s="605" t="s">
         <v>581</v>
@@ -25295,16 +25238,16 @@
     </row>
     <row r="47" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="49"/>
-      <c r="B47" s="673"/>
-      <c r="C47" s="674"/>
-      <c r="D47" s="673"/>
-      <c r="E47" s="674"/>
+      <c r="B47" s="678"/>
+      <c r="C47" s="679"/>
+      <c r="D47" s="678"/>
+      <c r="E47" s="679"/>
       <c r="F47" s="153" t="s">
         <v>38</v>
       </c>
       <c r="G47" s="153"/>
-      <c r="H47" s="675"/>
-      <c r="I47" s="674"/>
+      <c r="H47" s="680"/>
+      <c r="I47" s="679"/>
       <c r="J47" s="607" t="s">
         <v>172</v>
       </c>
@@ -25390,8 +25333,6 @@
       <c r="C53" s="90"/>
       <c r="D53" s="48"/>
       <c r="E53" s="90"/>
-      <c r="F53" s="0"/>
-      <c r="G53" s="0"/>
       <c r="H53" s="48"/>
       <c r="I53" s="90"/>
       <c r="J53" s="48"/>
@@ -25403,8 +25344,6 @@
       <c r="C54" s="598"/>
       <c r="D54" s="597"/>
       <c r="E54" s="598"/>
-      <c r="F54" s="0"/>
-      <c r="G54" s="0"/>
       <c r="H54" s="597"/>
       <c r="I54" s="598"/>
       <c r="J54" s="597"/>
@@ -25418,8 +25357,6 @@
       <c r="C55" s="37"/>
       <c r="D55" s="38"/>
       <c r="E55" s="37"/>
-      <c r="F55" s="0"/>
-      <c r="G55" s="0"/>
       <c r="H55" s="38"/>
       <c r="I55" s="37"/>
       <c r="J55" s="38"/>
@@ -25431,8 +25368,6 @@
       <c r="C56" s="598"/>
       <c r="D56" s="597"/>
       <c r="E56" s="598"/>
-      <c r="F56" s="0"/>
-      <c r="G56" s="0"/>
       <c r="H56" s="597"/>
       <c r="I56" s="598"/>
       <c r="J56" s="597"/>
@@ -25738,8 +25673,8 @@
   </sheetPr>
   <dimension ref="A2:O68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I28" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O46" activeCellId="1" sqref="S:S O46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O46" activeCellId="0" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25793,24 +25728,24 @@
         <v>2</v>
       </c>
       <c r="C4" s="586"/>
-      <c r="D4" s="639" t="s">
+      <c r="D4" s="644" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="639"/>
-      <c r="F4" s="639" t="s">
+      <c r="E4" s="644"/>
+      <c r="F4" s="644" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="639"/>
-      <c r="H4" s="676" t="s">
+      <c r="G4" s="644"/>
+      <c r="H4" s="681" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="676"/>
-      <c r="J4" s="676"/>
-      <c r="K4" s="639" t="s">
+      <c r="I4" s="681"/>
+      <c r="J4" s="681"/>
+      <c r="K4" s="644" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="639"/>
-      <c r="M4" s="639"/>
+      <c r="L4" s="644"/>
+      <c r="M4" s="644"/>
       <c r="O4" s="101"/>
     </row>
     <row r="5" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25847,7 +25782,7 @@
       <c r="E6" s="124"/>
       <c r="F6" s="433"/>
       <c r="G6" s="435"/>
-      <c r="H6" s="677" t="s">
+      <c r="H6" s="682" t="s">
         <v>602</v>
       </c>
       <c r="I6" s="141" t="s">
@@ -25970,7 +25905,7 @@
       <c r="K10" s="119" t="s">
         <v>78</v>
       </c>
-      <c r="L10" s="678" t="s">
+      <c r="L10" s="683" t="s">
         <v>167</v>
       </c>
       <c r="M10" s="124"/>
@@ -26026,7 +25961,7 @@
       <c r="K12" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="L12" s="678" t="s">
+      <c r="L12" s="683" t="s">
         <v>167</v>
       </c>
       <c r="M12" s="124"/>
@@ -26081,7 +26016,7 @@
       <c r="H14" s="119" t="s">
         <v>167</v>
       </c>
-      <c r="I14" s="678" t="s">
+      <c r="I14" s="683" t="s">
         <v>602</v>
       </c>
       <c r="J14" s="124" t="s">
@@ -26135,7 +26070,7 @@
       <c r="H16" s="59" t="s">
         <v>167</v>
       </c>
-      <c r="I16" s="678" t="s">
+      <c r="I16" s="683" t="s">
         <v>602</v>
       </c>
       <c r="J16" s="124" t="s">
@@ -26208,7 +26143,7 @@
       </c>
       <c r="B20" s="436"/>
       <c r="C20" s="438"/>
-      <c r="D20" s="679"/>
+      <c r="D20" s="684"/>
       <c r="E20" s="438"/>
       <c r="F20" s="436"/>
       <c r="G20" s="438"/>
@@ -26396,7 +26331,7 @@
       <c r="L31" s="603"/>
       <c r="M31" s="603"/>
       <c r="N31" s="603"/>
-      <c r="O31" s="631"/>
+      <c r="O31" s="636"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="70"/>
@@ -26463,7 +26398,7 @@
       <c r="M35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="646"/>
+      <c r="A36" s="651"/>
       <c r="B36" s="75" t="s">
         <v>2</v>
       </c>
@@ -26491,14 +26426,14 @@
       <c r="A37" s="594" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="665"/>
-      <c r="C37" s="666"/>
+      <c r="B37" s="670"/>
+      <c r="C37" s="671"/>
       <c r="D37" s="430"/>
       <c r="E37" s="198"/>
-      <c r="F37" s="680" t="s">
+      <c r="F37" s="685" t="s">
         <v>574</v>
       </c>
-      <c r="G37" s="680"/>
+      <c r="G37" s="685"/>
       <c r="H37" s="357"/>
       <c r="I37" s="357"/>
       <c r="J37" s="198"/>
@@ -26515,19 +26450,19 @@
     <row r="38" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="594"/>
       <c r="B38" s="171"/>
-      <c r="C38" s="669"/>
+      <c r="C38" s="674"/>
       <c r="D38" s="433"/>
       <c r="E38" s="199"/>
-      <c r="F38" s="681" t="s">
+      <c r="F38" s="686" t="s">
         <v>500</v>
       </c>
-      <c r="G38" s="681"/>
+      <c r="G38" s="686"/>
       <c r="J38" s="199"/>
-      <c r="K38" s="636" t="s">
+      <c r="K38" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L38" s="636"/>
-      <c r="M38" s="636"/>
+      <c r="L38" s="641"/>
+      <c r="M38" s="641"/>
       <c r="N38" s="81"/>
       <c r="O38" s="323"/>
     </row>
@@ -26539,14 +26474,14 @@
         <v>575</v>
       </c>
       <c r="C39" s="605"/>
-      <c r="D39" s="682" t="s">
+      <c r="D39" s="687" t="s">
         <v>689</v>
       </c>
-      <c r="E39" s="682"/>
-      <c r="F39" s="680" t="s">
+      <c r="E39" s="687"/>
+      <c r="F39" s="685" t="s">
         <v>574</v>
       </c>
-      <c r="G39" s="680"/>
+      <c r="G39" s="685"/>
       <c r="H39" s="529" t="s">
         <v>690</v>
       </c>
@@ -26572,20 +26507,20 @@
         <v>77</v>
       </c>
       <c r="E40" s="155"/>
-      <c r="F40" s="681" t="s">
+      <c r="F40" s="686" t="s">
         <v>500</v>
       </c>
-      <c r="G40" s="681"/>
+      <c r="G40" s="686"/>
       <c r="H40" s="621" t="s">
         <v>337</v>
       </c>
       <c r="I40" s="621"/>
       <c r="J40" s="621"/>
-      <c r="K40" s="636" t="s">
+      <c r="K40" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L40" s="636"/>
-      <c r="M40" s="636"/>
+      <c r="L40" s="641"/>
+      <c r="M40" s="641"/>
       <c r="N40" s="33"/>
       <c r="O40" s="33"/>
     </row>
@@ -26597,10 +26532,10 @@
         <v>575</v>
       </c>
       <c r="C41" s="605"/>
-      <c r="D41" s="682" t="s">
+      <c r="D41" s="687" t="s">
         <v>689</v>
       </c>
-      <c r="E41" s="682"/>
+      <c r="E41" s="687"/>
       <c r="F41" s="327" t="s">
         <v>692</v>
       </c>
@@ -26639,11 +26574,11 @@
       </c>
       <c r="I42" s="621"/>
       <c r="J42" s="621"/>
-      <c r="K42" s="636" t="s">
+      <c r="K42" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L42" s="636"/>
-      <c r="M42" s="636"/>
+      <c r="L42" s="641"/>
+      <c r="M42" s="641"/>
       <c r="N42" s="33"/>
       <c r="O42" s="33"/>
     </row>
@@ -26655,14 +26590,14 @@
         <v>581</v>
       </c>
       <c r="C43" s="605"/>
-      <c r="D43" s="657" t="s">
+      <c r="D43" s="662" t="s">
         <v>689</v>
       </c>
-      <c r="E43" s="657"/>
-      <c r="F43" s="683" t="s">
+      <c r="E43" s="662"/>
+      <c r="F43" s="688" t="s">
         <v>692</v>
       </c>
-      <c r="G43" s="683"/>
+      <c r="G43" s="688"/>
       <c r="H43" s="95" t="s">
         <v>690</v>
       </c>
@@ -26682,24 +26617,24 @@
         <v>172</v>
       </c>
       <c r="C44" s="607"/>
-      <c r="D44" s="684" t="s">
+      <c r="D44" s="689" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="684"/>
-      <c r="F44" s="684" t="s">
+      <c r="E44" s="689"/>
+      <c r="F44" s="689" t="s">
         <v>35</v>
       </c>
-      <c r="G44" s="684"/>
+      <c r="G44" s="689"/>
       <c r="H44" s="159" t="s">
         <v>77</v>
       </c>
       <c r="I44" s="159"/>
       <c r="J44" s="159"/>
-      <c r="K44" s="636" t="s">
+      <c r="K44" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L44" s="636"/>
-      <c r="M44" s="636"/>
+      <c r="L44" s="641"/>
+      <c r="M44" s="641"/>
       <c r="N44" s="33"/>
       <c r="O44" s="0"/>
     </row>
@@ -26711,14 +26646,14 @@
         <v>581</v>
       </c>
       <c r="C45" s="605"/>
-      <c r="D45" s="657" t="s">
+      <c r="D45" s="662" t="s">
         <v>689</v>
       </c>
-      <c r="E45" s="657"/>
-      <c r="F45" s="682" t="s">
+      <c r="E45" s="662"/>
+      <c r="F45" s="687" t="s">
         <v>692</v>
       </c>
-      <c r="G45" s="682"/>
+      <c r="G45" s="687"/>
       <c r="H45" s="95" t="s">
         <v>690</v>
       </c>
@@ -26740,10 +26675,10 @@
         <v>172</v>
       </c>
       <c r="C46" s="607"/>
-      <c r="D46" s="684" t="s">
+      <c r="D46" s="689" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="684"/>
+      <c r="E46" s="689"/>
       <c r="F46" s="155" t="s">
         <v>35</v>
       </c>
@@ -26753,11 +26688,11 @@
       </c>
       <c r="I46" s="159"/>
       <c r="J46" s="159"/>
-      <c r="K46" s="636" t="s">
+      <c r="K46" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L46" s="636"/>
-      <c r="M46" s="636"/>
+      <c r="L46" s="641"/>
+      <c r="M46" s="641"/>
       <c r="N46" s="81"/>
       <c r="O46" s="0"/>
     </row>
@@ -26769,10 +26704,10 @@
       <c r="C47" s="613"/>
       <c r="D47" s="38"/>
       <c r="E47" s="50"/>
-      <c r="F47" s="682" t="s">
+      <c r="F47" s="687" t="s">
         <v>692</v>
       </c>
-      <c r="G47" s="682"/>
+      <c r="G47" s="687"/>
       <c r="H47" s="36"/>
       <c r="I47" s="36"/>
       <c r="J47" s="37"/>
@@ -26788,8 +26723,8 @@
     </row>
     <row r="48" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="49"/>
-      <c r="B48" s="673"/>
-      <c r="C48" s="674"/>
+      <c r="B48" s="678"/>
+      <c r="C48" s="679"/>
       <c r="D48" s="23"/>
       <c r="E48" s="19"/>
       <c r="F48" s="159" t="s">
@@ -26799,11 +26734,11 @@
       <c r="H48" s="23"/>
       <c r="I48" s="18"/>
       <c r="J48" s="19"/>
-      <c r="K48" s="636" t="s">
+      <c r="K48" s="641" t="s">
         <v>172</v>
       </c>
-      <c r="L48" s="636"/>
-      <c r="M48" s="636"/>
+      <c r="L48" s="641"/>
+      <c r="M48" s="641"/>
       <c r="N48" s="81"/>
       <c r="O48" s="0"/>
     </row>
@@ -27188,8 +27123,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M13" activeCellId="1" sqref="S:S M13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27247,7 +27182,7 @@
       <c r="M3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="664"/>
+      <c r="A4" s="669"/>
       <c r="B4" s="246" t="s">
         <v>2</v>
       </c>
@@ -27256,14 +27191,14 @@
         <v>3</v>
       </c>
       <c r="E4" s="127"/>
-      <c r="F4" s="632" t="s">
+      <c r="F4" s="637" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="632"/>
-      <c r="H4" s="632" t="s">
+      <c r="G4" s="637"/>
+      <c r="H4" s="637" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="632"/>
+      <c r="I4" s="637"/>
       <c r="J4" s="593" t="s">
         <v>6</v>
       </c>
@@ -27510,17 +27445,17 @@
       <c r="M16" s="323"/>
     </row>
     <row r="17" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="685"/>
-      <c r="B17" s="685"/>
-      <c r="C17" s="685"/>
-      <c r="D17" s="685"/>
-      <c r="E17" s="685"/>
-      <c r="F17" s="685"/>
-      <c r="G17" s="685"/>
-      <c r="H17" s="685"/>
-      <c r="I17" s="685"/>
-      <c r="J17" s="685"/>
-      <c r="K17" s="685"/>
+      <c r="A17" s="690"/>
+      <c r="B17" s="690"/>
+      <c r="C17" s="690"/>
+      <c r="D17" s="690"/>
+      <c r="E17" s="690"/>
+      <c r="F17" s="690"/>
+      <c r="G17" s="690"/>
+      <c r="H17" s="690"/>
+      <c r="I17" s="690"/>
+      <c r="J17" s="690"/>
+      <c r="K17" s="690"/>
       <c r="L17" s="33"/>
       <c r="M17" s="323"/>
     </row>
@@ -27898,260 +27833,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:L22"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L22" activeCellId="1" sqref="S:S L22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.96"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="77" t="s">
-        <v>695</v>
-      </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="H1" s="77" t="s">
-        <v>696</v>
-      </c>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>697</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>698</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>697</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>699</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>699</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>699</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
-        <v>700</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>701</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>700</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
-        <v>702</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>703</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>702</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="0" t="s">
-        <v>704</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
-        <v>706</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>707</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
-        <v>708</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>709</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>708</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
-        <v>710</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>711</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>710</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
-        <v>712</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>713</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
-        <v>714</v>
-      </c>
-      <c r="I12" s="686" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>715</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
-        <v>716</v>
-      </c>
-      <c r="E14" s="686" t="s">
-        <v>717</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>716</v>
-      </c>
-      <c r="L14" s="686" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="686" t="s">
-        <v>718</v>
-      </c>
-      <c r="I15" s="686" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="686" t="s">
-        <v>719</v>
-      </c>
-      <c r="F16" s="686"/>
-      <c r="L16" s="686" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="686" t="n">
-        <v>4</v>
-      </c>
-      <c r="I17" s="686"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>720</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E19" s="0" t="s">
-        <v>721</v>
-      </c>
-      <c r="L19" s="0" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="0" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>723</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>724</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>725</v>
-      </c>
-      <c r="L22" s="0" t="s">
-        <v>726</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="H1:L1"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -28159,8 +27840,8 @@
   </sheetPr>
   <dimension ref="A2:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M14" activeCellId="1" sqref="S:S M14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29684,8 +29365,8 @@
   </sheetPr>
   <dimension ref="A2:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R58" activeCellId="1" sqref="S:S R58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R58" activeCellId="0" sqref="R58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31445,8 +31126,8 @@
   </sheetPr>
   <dimension ref="A2:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R54" activeCellId="1" sqref="S:S R54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R54" activeCellId="0" sqref="R54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33143,8 +32824,8 @@
   </sheetPr>
   <dimension ref="A2:N62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I40" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M58" activeCellId="1" sqref="S:S M58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I40" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M58" activeCellId="0" sqref="M58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34456,8 +34137,8 @@
   </sheetPr>
   <dimension ref="A2:S1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="1" sqref="S:S A35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36214,8 +35895,8 @@
   </sheetPr>
   <dimension ref="A2:S1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G26" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S42" activeCellId="0" sqref="S:S"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O37" activeCellId="0" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37982,8 +37663,8 @@
   </sheetPr>
   <dimension ref="A2:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L43" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R61" activeCellId="1" sqref="S:S R61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R61" activeCellId="0" sqref="R61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>